<commit_message>
Atualização na regra de negócio do formulário 03
</commit_message>
<xml_diff>
--- a/outputs/expansao_atualizado.xlsx
+++ b/outputs/expansao_atualizado.xlsx
@@ -8201,9 +8201,9 @@
           <t>Patricia Teixeira dos Santos</t>
         </is>
       </c>
-      <c r="E37" s="8" t="inlineStr">
-        <is>
-          <t>Enviado</t>
+      <c r="E37" s="18" t="inlineStr">
+        <is>
+          <t>Duplicado</t>
         </is>
       </c>
       <c r="F37" s="7" t="inlineStr">

</xml_diff>